<commit_message>
feat(CSVToAppComponent): CSV->AppComponent completed and tested.
</commit_message>
<xml_diff>
--- a/Protocol/src/ExcelToAppComponent/Eolian_fenix/components.xlsx
+++ b/Protocol/src/ExcelToAppComponent/Eolian_fenix/components.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ma\Documents\Github\Telemetria_Auriga\Protocol\src\ExcelToAppComponent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ma\Documents\Github\Telemetria_Auriga\Protocol\src\ExcelToAppComponent\Eolian_fenix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9206F41C-5F66-4993-9732-7C88FE76D316}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B03997-BCAE-4B66-9BB5-0A52E400E1AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="16080" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,8 +98,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -127,8 +135,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,10 +514,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D9F52BB-0BF4-4D49-892C-AB6869941B1B}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,7 +568,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>-0.1</v>
+        <v>-1</v>
       </c>
       <c r="B2">
         <v>-0.1</v>
@@ -645,7 +654,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>